<commit_message>
add jsons output folder
</commit_message>
<xml_diff>
--- a/scoring/forms/JRAQ/JRAQ93_test_1.xlsx
+++ b/scoring/forms/JRAQ/JRAQ93_test_1.xlsx
@@ -17,6 +17,8 @@
     <sheet name="outputs7" sheetId="8" state="visible" r:id="rId8"/>
     <sheet name="outputs8" sheetId="9" state="visible" r:id="rId9"/>
     <sheet name="outputs" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="outputs9" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="outputs10" sheetId="12" state="visible" r:id="rId12"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1" refMode="A1" iterate="0" iterateCount="100" iterateDelta="0.0001"/>
@@ -1099,112 +1101,148 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="3" t="inlineStr">
         <is>
           <t>پاسخ سیستم</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="3" t="inlineStr">
         <is>
           <t>پاسخ دستی کارشناس</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" s="3" t="inlineStr">
         <is>
           <t>clinical</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="A3" s="3" t="inlineStr">
         <is>
           <t>religious_ambivalence</t>
         </is>
       </c>
-      <c r="B3" t="n">
+      <c r="B3" s="3" t="n">
         <v>7</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
+      <c r="A4" s="3" t="inlineStr">
         <is>
           <t>religious_adherence</t>
         </is>
       </c>
-      <c r="B4" t="n">
+      <c r="B4" s="3" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
+      <c r="A5" s="3" t="inlineStr">
         <is>
           <t>religious_disobedience</t>
         </is>
       </c>
-      <c r="B5" t="n">
+      <c r="B5" s="3" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
+      <c r="A6" s="3" t="inlineStr">
         <is>
           <t>researchical</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
+      <c r="A7" s="3" t="inlineStr">
         <is>
           <t>religious_ambivalence</t>
         </is>
       </c>
-      <c r="B7" t="n">
+      <c r="B7" s="3" t="n">
         <v>24</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
+      <c r="A8" s="3" t="inlineStr">
         <is>
           <t>religious_adherence</t>
         </is>
       </c>
-      <c r="B8" t="n">
+      <c r="B8" s="3" t="n">
         <v>31</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
+      <c r="A9" s="3" t="inlineStr">
         <is>
           <t>religious_disobedience</t>
         </is>
       </c>
-      <c r="B9" t="n">
+      <c r="B9" s="3" t="n">
         <v>29</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
+      <c r="A10" s="3" t="inlineStr">
         <is>
           <t>clinical_raw</t>
         </is>
       </c>
-      <c r="B10" t="n">
+      <c r="B10" s="3" t="n">
         <v>30</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
+      <c r="A11" s="3" t="inlineStr">
         <is>
           <t>researchical_raw</t>
         </is>
       </c>
-      <c r="B11" t="n">
+      <c r="B11" s="3" t="n">
         <v>89</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>

</xml_diff>